<commit_message>
se actualiza versión en prod
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-AllergyIntoleranceInicioLE.xlsx
+++ b/docs/StructureDefinition-AllergyIntoleranceInicioLE.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>0.1.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-01-31T15:14:06-03:00</t>
+    <t>2023-02-10T14:01:31-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -770,7 +770,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://minsal.cl/listaespera/StructureDefinition/PacienteLE)
+    <t xml:space="preserve">Reference(http://minsal.cl/listaespera/StructureDefinition/PatientLE)
 </t>
   </si>
   <si>
@@ -1507,7 +1507,7 @@
     <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="64.51171875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="63.22265625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
update: se actualiza evento terminar(perfiles, ejemplos, información general)
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-AllergyIntoleranceInicioLE.xlsx
+++ b/docs/StructureDefinition-AllergyIntoleranceInicioLE.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-02-14T13:39:18-03:00</t>
+    <t>2023-02-15T12:48:14-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1497,17 +1497,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="42.24609375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="42.24609375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.1328125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="43.109375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="43.109375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="12.66015625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.9453125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="5.4296875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="63.22265625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="63.60546875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1516,25 +1516,25 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="8.84375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="120.87890625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="59.2890625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="39.51953125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="9.953125" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="17.171875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="124.42578125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="59.046875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="40.39453125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="11.0390625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="37" max="37" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="32.84375" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="43.93359375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="36.91796875" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="45.6171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
add: versión con evento inicio corregido v0.1.2
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-AllergyIntoleranceInicioLE.xlsx
+++ b/docs/StructureDefinition-AllergyIntoleranceInicioLE.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.1</t>
+    <t>0.1.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-11T07:17:50-03:00</t>
+    <t>2023-04-21T12:02:08-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1497,17 +1497,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="42.24609375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="42.24609375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.1328125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="43.109375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="43.109375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="12.66015625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.9453125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="5.4296875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="63.22265625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="63.60546875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1516,25 +1516,25 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="8.84375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="120.87890625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="59.2890625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="39.51953125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="9.953125" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="17.171875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="124.42578125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="59.046875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="40.39453125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="11.0390625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="37" max="37" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="32.84375" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="43.93359375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="36.91796875" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="45.6171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>